<commit_message>
final payment generator code
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>EMPLOYEE ID</t>
   </si>
@@ -31,124 +31,106 @@
     <t>DEDUCTIONS</t>
   </si>
   <si>
-    <t>Chipo Ndoro</t>
-  </si>
-  <si>
-    <t>chipondoro21@gmail.com</t>
-  </si>
-  <si>
-    <t>Tanyaradzwa Mhlauzi</t>
-  </si>
-  <si>
-    <t>tmhlauzi@gmail.com</t>
-  </si>
-  <si>
-    <t>Jasper Macherenga</t>
-  </si>
-  <si>
-    <t>juju36@gmail.com</t>
-  </si>
-  <si>
-    <t>Saseka Baloyi</t>
-  </si>
-  <si>
-    <t>sasekab00@gmail.com</t>
-  </si>
-  <si>
-    <t>Leon Nhiyo</t>
-  </si>
-  <si>
-    <t>nhiyonhyo01@gmail.com</t>
-  </si>
-  <si>
-    <t>Shalyne Madhoro</t>
-  </si>
-  <si>
-    <t>woobaby56@gmail.com</t>
-  </si>
-  <si>
-    <t>Tapiwa Matunya</t>
-  </si>
-  <si>
-    <t>matunyatapiwa@gmail.com</t>
-  </si>
-  <si>
-    <t>Tazvinga Muzire</t>
-  </si>
-  <si>
-    <t>muziretazvinga67@gmail.com</t>
-  </si>
-  <si>
-    <t>Malvin Tafirenyika</t>
-  </si>
-  <si>
-    <t>malvinofficial@gmail.com</t>
-  </si>
-  <si>
-    <t>George Bishi</t>
-  </si>
-  <si>
-    <t>george4567@gmail.com</t>
-  </si>
-  <si>
-    <t>Dean Mugwagwa</t>
-  </si>
-  <si>
-    <t>deannhunhu12@gmail.com</t>
-  </si>
-  <si>
-    <t>Sean Mangwanya</t>
-  </si>
-  <si>
-    <t>mangwanya654@gmail.com</t>
-  </si>
-  <si>
-    <t>Peter Munyingwa</t>
-  </si>
-  <si>
-    <t>peter2458@gmail.com</t>
-  </si>
-  <si>
-    <t>Andrew Monday</t>
-  </si>
-  <si>
-    <t>andrewmonday@gmail.com</t>
-  </si>
-  <si>
-    <t>owen Gohva</t>
-  </si>
-  <si>
-    <t>owensungo54@gmail.com</t>
-  </si>
-  <si>
-    <t>Amanda Sungo</t>
-  </si>
-  <si>
-    <t>amandasungo98@gmail.com</t>
-  </si>
-  <si>
-    <t>Olen Mupedzanhamo</t>
-  </si>
-  <si>
-    <t>olenmapedzanhamo45@gmail.com</t>
-  </si>
-  <si>
-    <t>Takudzwa Ndangana</t>
-  </si>
-  <si>
-    <t>takudzwandangana@gmail.com</t>
-  </si>
-  <si>
-    <t>John Hungwe</t>
-  </si>
-  <si>
-    <t>johnhungwe45@gmail.com</t>
-  </si>
-  <si>
-    <t>Thomas Ngwena</t>
-  </si>
-  <si>
-    <t>thomasngwenya67@gmail.com</t>
+    <t>Loe Mazive</t>
+  </si>
+  <si>
+    <t>leomazive01@gmail.com</t>
+  </si>
+  <si>
+    <t>Craig Togarepi</t>
+  </si>
+  <si>
+    <t>craigtogs@gmail.com</t>
+  </si>
+  <si>
+    <t>Nyasha Zimbudzana</t>
+  </si>
+  <si>
+    <t>nyashazee07@gmail.com</t>
+  </si>
+  <si>
+    <t>Verna Dumbatsuro</t>
+  </si>
+  <si>
+    <t>vdumbatsuro2@gmail.com</t>
+  </si>
+  <si>
+    <t>Haille Mashiri</t>
+  </si>
+  <si>
+    <t>haillemashiri05@gmail.com</t>
+  </si>
+  <si>
+    <t>James Mutembedza</t>
+  </si>
+  <si>
+    <t>jamesmutembedza87@gmail.com</t>
+  </si>
+  <si>
+    <t>Russell  Chipunza</t>
+  </si>
+  <si>
+    <t>russell2.0c@gmail.com</t>
+  </si>
+  <si>
+    <t>Lovemore Kugarauswa</t>
+  </si>
+  <si>
+    <t>lovemoreheila@gmail.com</t>
+  </si>
+  <si>
+    <t>Lorreine Dumbatsuro</t>
+  </si>
+  <si>
+    <t>ldumbatsuro6@gmail.com</t>
+  </si>
+  <si>
+    <t>Tapiwa Mwedzi</t>
+  </si>
+  <si>
+    <t>tapiwamwedzi7@gmail.com</t>
+  </si>
+  <si>
+    <t>Covenent mapuranga</t>
+  </si>
+  <si>
+    <t>mapurangacovenant1@gmail.com</t>
+  </si>
+  <si>
+    <t>Roshly Musonza</t>
+  </si>
+  <si>
+    <t>musonzaroshly@gmail.com</t>
+  </si>
+  <si>
+    <t>Tanatswa Lionde</t>
+  </si>
+  <si>
+    <t>liondetanatswa@gmail.com</t>
+  </si>
+  <si>
+    <t>Fredson Matosi</t>
+  </si>
+  <si>
+    <t>TiritoseUekela@gmail.com</t>
+  </si>
+  <si>
+    <t>Tabani Tytem</t>
+  </si>
+  <si>
+    <t>Ttytem@gmail.com</t>
+  </si>
+  <si>
+    <t>Joseph Mutembedza</t>
+  </si>
+  <si>
+    <t>jamesmutembedza@gmail.com</t>
+  </si>
+  <si>
+    <t>Tapiwa Ndemera</t>
+  </si>
+  <si>
+    <t>tapiwandemera@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -191,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -202,6 +184,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -786,64 +771,14 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
-        <v>2571.0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="2">
-        <v>600.0</v>
-      </c>
-      <c r="E19" s="2">
-        <v>250.0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>121.0</v>
-      </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="2">
-        <v>1834.0</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="2">
-        <v>450.0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>150.0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>98.0</v>
-      </c>
+      <c r="C20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="2">
-        <v>6038.0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="2">
-        <v>250.0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>85.0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>55.0</v>
-      </c>
+      <c r="C21" s="4"/>
+      <c r="F21" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -864,10 +799,7 @@
     <hyperlink r:id="rId15" ref="C16"/>
     <hyperlink r:id="rId16" ref="C17"/>
     <hyperlink r:id="rId17" ref="C18"/>
-    <hyperlink r:id="rId18" ref="C19"/>
-    <hyperlink r:id="rId19" ref="C20"/>
-    <hyperlink r:id="rId20" ref="C21"/>
   </hyperlinks>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>